<commit_message>
added basic course files
</commit_message>
<xml_diff>
--- a/beginner-grammar/tenses.xlsx
+++ b/beginner-grammar/tenses.xlsx
@@ -73,7 +73,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Суб'єкт + Дієслово (v1)
+      <t xml:space="preserve">Суб'єкт + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -93,7 +114,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">I work at home.
+      <t xml:space="preserve">I </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> at home.
 </t>
     </r>
     <r>
@@ -133,7 +175,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Суб'єкт + Дієслово (v1) + </t>
+      <t xml:space="preserve">Суб'єкт + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -165,7 +228,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">She think</t>
+      <t xml:space="preserve">She </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
     </r>
     <r>
       <rPr>
@@ -188,7 +262,18 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> ahead.
-            He do</t>
+            He </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">do</t>
     </r>
     <r>
       <rPr>
@@ -250,7 +335,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Суб'єкт + Дієслово (v1)
+      <t xml:space="preserve">Суб'єкт + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -270,7 +376,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">We spend time here.</t>
+      <t xml:space="preserve">We </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> time here.</t>
     </r>
   </si>
   <si>
@@ -323,7 +450,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -377,7 +525,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -461,7 +620,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -515,7 +695,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
     </r>
     <r>
       <rPr>
@@ -579,7 +770,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> do</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">do</t>
     </r>
     <r>
       <rPr>
@@ -663,7 +865,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -717,7 +940,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spend</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
     </r>
     <r>
       <rPr>
@@ -792,7 +1026,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -825,7 +1080,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -900,7 +1166,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -942,7 +1229,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> thought ahead.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">thought</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ahead.
 </t>
     </r>
     <r>
@@ -984,7 +1292,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> done it well.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">done</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> it well.
 </t>
     </r>
     <r>
@@ -1046,7 +1375,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -1088,7 +1438,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spent time here.</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spent</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> time here.</t>
     </r>
   </si>
   <si>
@@ -1141,7 +1512,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -1186,7 +1578,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -1261,7 +1664,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -1315,7 +1739,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
     </r>
     <r>
       <rPr>
@@ -1375,6 +1810,7 @@
       <rPr>
         <i val="true"/>
         <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Ubuntu Mono"/>
         <family val="0"/>
         <charset val="1"/>
@@ -1463,7 +1899,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -1517,7 +1974,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spend</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
     </r>
     <r>
       <rPr>
@@ -1574,7 +2042,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Суб'єкт + Дієслово (v2)
+      <t xml:space="preserve">Суб'єкт + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v2</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -1594,7 +2083,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">I work</t>
+      <t xml:space="preserve">I </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -1656,7 +2156,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Суб'єкт + Дієслово (v2)
+      <t xml:space="preserve">Суб'єкт + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v2</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -1676,8 +2197,50 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">She thought ahead.
-            He did it well.
+      <t xml:space="preserve">She </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">thought</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ahead.
+            He </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">did</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> it well.
 </t>
     </r>
     <r>
@@ -1717,7 +2280,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Суб'єкт + Дієслово (v2)
+      <t xml:space="preserve">Суб'єкт + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v2</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -1737,7 +2321,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">We spent time here.</t>
+      <t xml:space="preserve">We </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spent</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> time here.</t>
     </r>
   </si>
   <si>
@@ -1790,7 +2395,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -1844,7 +2470,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -1928,7 +2565,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -1982,7 +2640,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
     </r>
     <r>
       <rPr>
@@ -2046,7 +2715,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> do</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">do</t>
     </r>
     <r>
       <rPr>
@@ -2130,7 +2810,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -2184,7 +2885,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spend</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
     </r>
     <r>
       <rPr>
@@ -2259,7 +2971,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -2292,7 +3025,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -2367,7 +3111,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -2409,7 +3174,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> thought ahead.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">thought</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ahead.
 </t>
     </r>
     <r>
@@ -2451,7 +3237,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> done it well.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">done</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> it well.
 </t>
     </r>
     <r>
@@ -2513,7 +3320,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -2555,7 +3383,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spent time here.</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spent</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> time here.</t>
     </r>
   </si>
   <si>
@@ -2608,7 +3457,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -2653,7 +3523,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -2728,7 +3609,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -2782,7 +3684,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
     </r>
     <r>
       <rPr>
@@ -2842,6 +3755,7 @@
       <rPr>
         <i val="true"/>
         <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Ubuntu Mono"/>
         <family val="0"/>
         <charset val="1"/>
@@ -2930,7 +3844,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -2984,7 +3919,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spend</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
     </r>
     <r>
       <rPr>
@@ -3063,7 +4009,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -3105,7 +4072,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work at home.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> at home.
 </t>
     </r>
     <r>
@@ -3167,7 +4155,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -3209,7 +4218,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think ahead.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ahead.
             He </t>
     </r>
     <r>
@@ -3228,11 +4258,22 @@
       <rPr>
         <i val="true"/>
         <sz val="10"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">do it well.
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">do</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> it well.
 </t>
     </r>
     <r>
@@ -3294,7 +4335,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -3389,7 +4451,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -3443,7 +4526,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -3527,7 +4621,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -3581,7 +4696,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
     </r>
     <r>
       <rPr>
@@ -3645,7 +4771,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> do</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">do</t>
     </r>
     <r>
       <rPr>
@@ -3729,7 +4866,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -3783,7 +4941,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spend</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
     </r>
     <r>
       <rPr>
@@ -3858,7 +5027,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -3891,7 +5081,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -3966,7 +5167,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -4050,7 +5272,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> done it well.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">done</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> it well.
 </t>
     </r>
     <r>
@@ -4112,7 +5355,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -4154,7 +5418,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spent time here.</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spent</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> time here.</t>
     </r>
   </si>
   <si>
@@ -4207,7 +5492,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -4252,7 +5558,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -4327,7 +5644,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -4381,7 +5719,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
     </r>
     <r>
       <rPr>
@@ -4441,6 +5790,7 @@
       <rPr>
         <i val="true"/>
         <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Ubuntu Mono"/>
         <family val="0"/>
         <charset val="1"/>
@@ -4529,7 +5879,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -4583,7 +5954,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spend</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
     </r>
     <r>
       <rPr>
@@ -4662,7 +6044,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -4704,7 +6107,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work at home.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> at home.
 </t>
     </r>
     <r>
@@ -4766,7 +6190,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -4808,7 +6253,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think ahead.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ahead.
             He </t>
     </r>
     <r>
@@ -4827,11 +6293,22 @@
       <rPr>
         <i val="true"/>
         <sz val="10"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">do it well.
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">do</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> it well.
 </t>
     </r>
     <r>
@@ -4893,7 +6370,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -4931,11 +6429,22 @@
       <rPr>
         <i val="true"/>
         <sz val="10"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">spend time here.</t>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> time here.</t>
     </r>
   </si>
   <si>
@@ -4988,7 +6497,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -5042,7 +6572,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -5126,7 +6667,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -5180,7 +6742,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
     </r>
     <r>
       <rPr>
@@ -5244,7 +6817,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> do</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">do</t>
     </r>
     <r>
       <rPr>
@@ -5328,7 +6912,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -5382,7 +6987,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spend</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
     </r>
     <r>
       <rPr>
@@ -5457,7 +7073,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -5490,7 +7127,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -5565,7 +7213,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -5607,7 +7276,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> thought ahead.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">thought</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ahead.
 </t>
     </r>
     <r>
@@ -5649,7 +7339,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> done it well.
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">done</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> it well.
 </t>
     </r>
     <r>
@@ -5711,7 +7422,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v3)
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v3</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
     </r>
     <r>
@@ -5753,7 +7485,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spent time here.</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FF2A6099"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spent</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> time here.</t>
     </r>
   </si>
   <si>
@@ -5806,7 +7559,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -5851,7 +7625,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> work</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
     </r>
     <r>
       <rPr>
@@ -5926,7 +7711,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -5980,7 +7786,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> think</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">think</t>
     </r>
     <r>
       <rPr>
@@ -6040,6 +7857,7 @@
       <rPr>
         <i val="true"/>
         <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Ubuntu Mono"/>
         <family val="0"/>
         <charset val="1"/>
@@ -6128,7 +7946,28 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> + Дієслово (v1) + </t>
+      <t xml:space="preserve"> + Дієслово (</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v1</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) + </t>
     </r>
     <r>
       <rPr>
@@ -6182,7 +8021,18 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> spend</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">spend</t>
     </r>
     <r>
       <rPr>
@@ -6215,7 +8065,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -6265,8 +8115,24 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Ubuntu Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="10"/>
+      <name val="Ubuntu Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Ubuntu Mono"/>
       <family val="0"/>
       <charset val="1"/>
@@ -6285,6 +8151,38 @@
       <i val="true"/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Ubuntu Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF2A6099"/>
+      <name val="Ubuntu Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF2A6099"/>
+      <name val="Ubuntu Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF00A933"/>
+      <name val="Ubuntu Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF00A933"/>
       <name val="Ubuntu Mono"/>
       <family val="0"/>
       <charset val="1"/>
@@ -6352,7 +8250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6373,15 +8271,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6394,6 +8288,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF2A6099"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -6404,15 +8358,16 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B2" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="64.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="64.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="64.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="64.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6488,7 +8443,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="107.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -6505,11 +8460,11 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>